<commit_message>
se modifica plantilla de servicos
</commit_message>
<xml_diff>
--- a/src/assets/archivos/Plantilla_estandar_para_cargar_servicios.xlsx
+++ b/src/assets/archivos/Plantilla_estandar_para_cargar_servicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF29F4E0-5E37-4499-99E7-9328A48A6770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC1C1BA-A3EF-42F7-9F7C-47D1B9FCE142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F63BF03C-E539-45D8-A7A9-6EBB3DC6BF4F}"/>
   </bookViews>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8E60EC-58D0-49D4-8E8A-104F4D8A18CE}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,24 +550,18 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione" xr:uid="{C557888B-4E9F-4B0F-B4C3-CF3FCF95F3F8}">
           <x14:formula1>
             <xm:f>Desplegables!$A$2:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>E3:E102</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione" xr:uid="{906863C2-0B2D-4963-81D1-10A91E43E33B}">
-          <x14:formula1>
-            <xm:f>Desplegables!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>F4:F102</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione" xr:uid="{4C7EA23F-AF30-4A53-B680-8703C0B07737}">
           <x14:formula1>
             <xm:f>Desplegables!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F3</xm:sqref>
+          <xm:sqref>F3:F134</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>